<commit_message>
Working towards excel template upload
</commit_message>
<xml_diff>
--- a/public/GearGoober Equipment Template.xlsx
+++ b/public/GearGoober Equipment Template.xlsx
@@ -24,24 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Kit Name</t>
-  </si>
-  <si>
-    <t>Kit Parent</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Comma Separated Barcodes List</t>
   </si>
   <si>
-    <t>(If piece of equipment is in a kit)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Expanations: </t>
-  </si>
-  <si>
-    <t>(If the kit is within a kit)</t>
   </si>
   <si>
     <t>Equip Manufacturer Name</t>
@@ -70,13 +58,7 @@
 category of Audio)</t>
   </si>
   <si>
-    <t>Kit Category</t>
-  </si>
-  <si>
     <t>(If the equipment is in a kit, the category may be "Kit Items")</t>
-  </si>
-  <si>
-    <t>Kit Category Parent</t>
   </si>
 </sst>
 </file>
@@ -417,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,65 +414,43 @@
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>